<commit_message>
Updated prefab and wiring spreadsheets.
Updated prefab wiring to reflect newly-built cables. Corrected errors in
wiring spreadsheet.
</commit_message>
<xml_diff>
--- a/2013_Wiring.xlsx
+++ b/2013_Wiring.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\Documents\GitHub\FRC2994_2013_Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="666"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="666" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Power Distribution Board" sheetId="1" r:id="rId1"/>
@@ -16,12 +21,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'PWM Cables'!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="175">
   <si>
     <t>2013 TEAM 2994</t>
   </si>
@@ -170,18 +175,12 @@
     <t>PWM8</t>
   </si>
   <si>
-    <t>DIO12</t>
-  </si>
-  <si>
     <t>Shooter Jag</t>
   </si>
   <si>
     <t>PWM7</t>
   </si>
   <si>
-    <t>DIO11</t>
-  </si>
-  <si>
     <t>Right Arm Talon 2 (J6)</t>
   </si>
   <si>
@@ -552,12 +551,6 @@
   </si>
   <si>
     <t>Shooter M/C (J7)</t>
-  </si>
-  <si>
-    <t>Shooter Encoder B</t>
-  </si>
-  <si>
-    <t>Shooter Encoder A</t>
   </si>
 </sst>
 </file>
@@ -1207,21 +1200,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1276,6 +1254,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1355,6 +1348,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1678,7 +1674,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1713,7 +1709,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1927,8 +1923,8 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +1963,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1986,35 +1982,35 @@
       <c r="K4" s="47"/>
     </row>
     <row r="5" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="55"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="35"/>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="56"/>
+      <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="61" t="s">
-        <v>167</v>
+      <c r="A6" s="56" t="s">
+        <v>165</v>
       </c>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
       <c r="D6" s="35"/>
       <c r="J6" s="37"/>
       <c r="K6" s="48"/>
-      <c r="L6" s="61" t="s">
+      <c r="L6" s="56" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="57">
+        <v>31</v>
+      </c>
+      <c r="B7" s="55" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="62">
-        <v>31</v>
-      </c>
-      <c r="B7" s="60" t="s">
-        <v>169</v>
       </c>
       <c r="C7" s="53" t="s">
         <v>4</v>
@@ -2024,18 +2020,18 @@
         <v>5</v>
       </c>
       <c r="K7" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="L7" s="62">
+        <v>171</v>
+      </c>
+      <c r="L7" s="57">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62">
+      <c r="A8" s="57">
         <v>30</v>
       </c>
-      <c r="B8" s="60" t="s">
-        <v>170</v>
+      <c r="B8" s="55" t="s">
+        <v>168</v>
       </c>
       <c r="C8" s="53" t="s">
         <v>8</v>
@@ -2045,18 +2041,18 @@
         <v>9</v>
       </c>
       <c r="K8" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="L8" s="62">
+        <v>172</v>
+      </c>
+      <c r="L8" s="57">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62">
+      <c r="A9" s="57">
         <v>29</v>
       </c>
-      <c r="B9" s="60" t="s">
-        <v>171</v>
+      <c r="B9" s="55" t="s">
+        <v>169</v>
       </c>
       <c r="C9" s="53" t="s">
         <v>11</v>
@@ -2066,18 +2062,18 @@
         <v>12</v>
       </c>
       <c r="K9" s="50" t="s">
-        <v>175</v>
-      </c>
-      <c r="L9" s="62">
+        <v>173</v>
+      </c>
+      <c r="L9" s="57">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="62">
+      <c r="A10" s="57">
         <v>28</v>
       </c>
-      <c r="B10" s="60" t="s">
-        <v>172</v>
+      <c r="B10" s="55" t="s">
+        <v>170</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>14</v>
@@ -2087,17 +2083,17 @@
         <v>15</v>
       </c>
       <c r="K10" s="51" t="s">
-        <v>176</v>
-      </c>
-      <c r="L10" s="62">
+        <v>174</v>
+      </c>
+      <c r="L10" s="57">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62">
+      <c r="A11" s="57">
         <v>27</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="55" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="53" t="s">
@@ -2108,11 +2104,11 @@
         <v>19</v>
       </c>
       <c r="K11" s="50"/>
-      <c r="L11" s="62"/>
+      <c r="L11" s="57"/>
     </row>
     <row r="12" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
-      <c r="B12" s="60"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="53" t="s">
         <v>20</v>
       </c>
@@ -2121,11 +2117,11 @@
         <v>21</v>
       </c>
       <c r="K12" s="50"/>
-      <c r="L12" s="62"/>
+      <c r="L12" s="57"/>
     </row>
     <row r="13" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
-      <c r="B13" s="60"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="53" t="s">
         <v>22</v>
       </c>
@@ -2134,13 +2130,13 @@
         <v>23</v>
       </c>
       <c r="K13" s="50"/>
-      <c r="L13" s="62"/>
+      <c r="L13" s="57"/>
     </row>
     <row r="14" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62">
+      <c r="A14" s="57">
         <v>26</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="55" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="53" t="s">
@@ -2151,13 +2147,13 @@
         <v>26</v>
       </c>
       <c r="K14" s="50"/>
-      <c r="L14" s="62"/>
+      <c r="L14" s="57"/>
     </row>
     <row r="15" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62">
+      <c r="A15" s="57">
         <v>25</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="55" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="53" t="s">
@@ -2168,31 +2164,31 @@
         <v>29</v>
       </c>
       <c r="K15" s="50"/>
-      <c r="L15" s="62"/>
+      <c r="L15" s="57"/>
     </row>
     <row r="16" spans="1:12" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63">
+      <c r="A16" s="58">
         <v>24</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="68" t="s">
+      <c r="D16" s="61"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="69" t="s">
-        <v>168</v>
-      </c>
-      <c r="L16" s="63">
+      <c r="K16" s="64" t="s">
+        <v>166</v>
+      </c>
+      <c r="L16" s="58">
         <v>36</v>
       </c>
     </row>
@@ -2233,13 +2229,13 @@
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
-      <c r="E20" s="81">
+      <c r="E20" s="76">
         <v>38</v>
       </c>
-      <c r="F20" s="81">
+      <c r="F20" s="76">
         <v>37</v>
       </c>
-      <c r="G20" s="81" t="s">
+      <c r="G20" s="76" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2267,8 +2263,8 @@
   </sheetPr>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,7 +2284,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1"/>
@@ -2382,13 +2378,13 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
-      <c r="K14" s="73" t="s">
-        <v>167</v>
+      <c r="K14" s="68" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
-        <v>167</v>
+      <c r="A15" s="68" t="s">
+        <v>165</v>
       </c>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
@@ -2402,15 +2398,15 @@
       <c r="I15" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="70"/>
-      <c r="K15" s="74"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="69"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="74">
+      <c r="A16" s="69">
         <v>6</v>
       </c>
-      <c r="B16" s="71" t="s">
-        <v>159</v>
+      <c r="B16" s="66" t="s">
+        <v>157</v>
       </c>
       <c r="C16" s="36" t="s">
         <v>42</v>
@@ -2425,11 +2421,11 @@
       <c r="I16" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="J16" s="70"/>
-      <c r="K16" s="74"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="69"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="75"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="35"/>
@@ -2437,15 +2433,9 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
-      <c r="I17" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="70" t="s">
-        <v>177</v>
-      </c>
-      <c r="K17" s="77">
-        <v>10</v>
-      </c>
+      <c r="I17" s="40"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="72"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
@@ -2456,17 +2446,13 @@
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
-      <c r="I18" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="J18" s="70" t="s">
-        <v>178</v>
-      </c>
-      <c r="K18" s="77"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="72"/>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="74"/>
-      <c r="B19" s="71"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="66"/>
       <c r="C19" s="36" t="s">
         <v>45</v>
       </c>
@@ -2478,10 +2464,10 @@
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
       <c r="I19" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="74"/>
+        <v>53</v>
+      </c>
+      <c r="J19" s="65"/>
+      <c r="K19" s="69"/>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26"/>
@@ -2493,16 +2479,16 @@
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
       <c r="I20" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="J20" s="70"/>
-      <c r="K20" s="74"/>
+        <v>56</v>
+      </c>
+      <c r="J20" s="65"/>
+      <c r="K20" s="69"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="74">
+      <c r="A21" s="69">
         <v>5</v>
       </c>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="66" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="36" t="s">
@@ -2516,17 +2502,17 @@
       <c r="G21" s="37"/>
       <c r="H21" s="37"/>
       <c r="I21" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="J21" s="70" t="s">
-        <v>61</v>
-      </c>
-      <c r="K21" s="74">
+        <v>58</v>
+      </c>
+      <c r="J21" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="69">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="75"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
       <c r="D22" s="37"/>
@@ -2535,12 +2521,12 @@
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
       <c r="I22" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="J22" s="70" t="s">
-        <v>64</v>
-      </c>
-      <c r="K22" s="74">
+        <v>61</v>
+      </c>
+      <c r="J22" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" s="69">
         <v>15</v>
       </c>
     </row>
@@ -2554,24 +2540,24 @@
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
       <c r="I23" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="J23" s="70" t="s">
-        <v>161</v>
-      </c>
-      <c r="K23" s="74">
+        <v>64</v>
+      </c>
+      <c r="J23" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="K23" s="69">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="74">
+      <c r="A24" s="69">
         <v>4</v>
       </c>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="36" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" s="36" t="s">
-        <v>51</v>
       </c>
       <c r="D24" s="39" t="s">
         <v>43</v>
@@ -2581,17 +2567,17 @@
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
       <c r="I24" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="J24" s="70" t="s">
-        <v>160</v>
-      </c>
-      <c r="K24" s="74">
+        <v>66</v>
+      </c>
+      <c r="J24" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="K24" s="69">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
@@ -2600,13 +2586,13 @@
       <c r="G25" s="37"/>
       <c r="H25" s="37"/>
       <c r="I25" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="J25" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="K25" s="77">
-        <v>11</v>
+        <v>67</v>
+      </c>
+      <c r="J25" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" s="72">
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2619,18 +2605,20 @@
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
       <c r="I26" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="J26" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="K26" s="77"/>
+        <v>69</v>
+      </c>
+      <c r="J26" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" s="72">
+        <v>81</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="74"/>
-      <c r="B27" s="71"/>
+      <c r="A27" s="69"/>
+      <c r="B27" s="66"/>
       <c r="C27" s="36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D27" s="39" t="s">
         <v>43</v>
@@ -2640,17 +2628,17 @@
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
       <c r="I27" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="J27" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="K27" s="77">
-        <v>9</v>
+        <v>71</v>
+      </c>
+      <c r="J27" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" s="72">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="75"/>
+      <c r="A28" s="70"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
@@ -2659,12 +2647,14 @@
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
       <c r="I28" s="40" t="s">
-        <v>75</v>
-      </c>
-      <c r="J28" s="70" t="s">
-        <v>76</v>
-      </c>
-      <c r="K28" s="78"/>
+        <v>73</v>
+      </c>
+      <c r="J28" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="K28" s="73">
+        <v>91</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30"/>
@@ -2678,14 +2668,14 @@
       <c r="K29" s="24"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="74">
+      <c r="A30" s="69">
         <v>3</v>
       </c>
-      <c r="B30" s="71" t="s">
-        <v>158</v>
+      <c r="B30" s="66" t="s">
+        <v>156</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D30" s="39" t="s">
         <v>43</v>
@@ -2708,10 +2698,10 @@
       <c r="K31" s="24"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="74"/>
-      <c r="B32" s="71"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="66"/>
       <c r="C32" s="36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="39" t="s">
         <v>43</v>
@@ -2721,13 +2711,13 @@
       <c r="G32" s="37"/>
       <c r="H32" s="37"/>
       <c r="I32" s="40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J32" s="7"/>
-      <c r="K32" s="73"/>
+      <c r="K32" s="68"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="75"/>
+      <c r="A33" s="70"/>
       <c r="B33" s="35"/>
       <c r="C33" s="35"/>
       <c r="D33" s="35"/>
@@ -2736,10 +2726,10 @@
       <c r="G33" s="37"/>
       <c r="H33" s="37"/>
       <c r="I33" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J33" s="7"/>
-      <c r="K33" s="74"/>
+      <c r="K33" s="69"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30"/>
@@ -2751,20 +2741,20 @@
       <c r="G34" s="37"/>
       <c r="H34" s="37"/>
       <c r="I34" s="40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J34" s="7"/>
-      <c r="K34" s="74"/>
+      <c r="K34" s="69"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="74">
+      <c r="A35" s="69">
         <v>2</v>
       </c>
-      <c r="B35" s="71" t="s">
-        <v>157</v>
+      <c r="B35" s="66" t="s">
+        <v>155</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D35" s="39" t="s">
         <v>43</v>
@@ -2774,13 +2764,13 @@
       <c r="G35" s="37"/>
       <c r="H35" s="37"/>
       <c r="I35" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J35" s="7"/>
-      <c r="K35" s="74"/>
+      <c r="K35" s="69"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="75"/>
+      <c r="A36" s="70"/>
       <c r="B36" s="35"/>
       <c r="C36" s="35"/>
       <c r="D36" s="35"/>
@@ -2789,10 +2779,10 @@
       <c r="G36" s="37"/>
       <c r="H36" s="37"/>
       <c r="I36" s="40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J36" s="7"/>
-      <c r="K36" s="74"/>
+      <c r="K36" s="69"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30"/>
@@ -2804,16 +2794,16 @@
       <c r="G37" s="37"/>
       <c r="H37" s="37"/>
       <c r="I37" s="40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J37" s="7"/>
-      <c r="K37" s="74"/>
+      <c r="K37" s="69"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="74"/>
-      <c r="B38" s="71"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="66"/>
       <c r="C38" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" s="39" t="s">
         <v>43</v>
@@ -2823,17 +2813,17 @@
       <c r="G38" s="37"/>
       <c r="H38" s="37"/>
       <c r="I38" s="40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K38" s="74">
-        <v>8</v>
+        <v>82</v>
+      </c>
+      <c r="K38" s="69">
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="75"/>
+      <c r="A39" s="70"/>
       <c r="B39" s="35"/>
       <c r="C39" s="35"/>
       <c r="D39" s="35"/>
@@ -2842,12 +2832,12 @@
       <c r="G39" s="37"/>
       <c r="H39" s="37"/>
       <c r="I39" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="K39" s="76">
+        <v>84</v>
+      </c>
+      <c r="K39" s="71">
         <v>7</v>
       </c>
     </row>
@@ -2862,14 +2852,14 @@
       <c r="H40" s="37"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="76">
+      <c r="A41" s="71">
         <v>1</v>
       </c>
-      <c r="B41" s="71" t="s">
-        <v>156</v>
+      <c r="B41" s="66" t="s">
+        <v>154</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D41" s="39" t="s">
         <v>43</v>
@@ -2950,34 +2940,29 @@
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F53" s="41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G53" s="41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F54" s="41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G54" s="41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F55" s="81">
+      <c r="F55" s="76">
         <v>24</v>
       </c>
-      <c r="G55" s="81">
+      <c r="G55" s="76">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="K27:K28"/>
-  </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup scale="62" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
@@ -3014,43 +2999,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
+      <c r="B2" s="81" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
       <c r="N2" s="8"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
       <c r="F4" s="44"/>
       <c r="I4" s="44" t="s">
         <v>27</v>
@@ -3064,7 +3049,7 @@
         <v>41</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="37"/>
@@ -3075,10 +3060,10 @@
     </row>
     <row r="7" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="37"/>
@@ -3090,7 +3075,7 @@
     <row r="8" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="18"/>
       <c r="D8" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="37"/>
@@ -3100,182 +3085,182 @@
       <c r="K8" s="17"/>
     </row>
     <row r="9" spans="2:14" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="61" t="s">
-        <v>167</v>
+      <c r="B9" s="56" t="s">
+        <v>165</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
       <c r="E9" s="17"/>
       <c r="F9" s="37"/>
-      <c r="H9" s="73" t="s">
-        <v>167</v>
+      <c r="H9" s="68" t="s">
+        <v>165</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="19"/>
       <c r="K9" s="17"/>
     </row>
     <row r="10" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="62"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="37"/>
-      <c r="H10" s="74"/>
+      <c r="H10" s="69"/>
       <c r="I10" s="5"/>
       <c r="J10" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K10" s="17"/>
     </row>
     <row r="11" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="62"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="37"/>
-      <c r="H11" s="74"/>
+      <c r="H11" s="69"/>
       <c r="I11" s="5"/>
       <c r="J11" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K11" s="17"/>
     </row>
     <row r="12" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="62"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="37"/>
-      <c r="H12" s="74">
+      <c r="H12" s="69">
         <v>23</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K12" s="17"/>
     </row>
     <row r="13" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="62">
+      <c r="B13" s="57">
         <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="37"/>
-      <c r="H13" s="74">
+      <c r="H13" s="69">
         <v>22</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K13" s="17"/>
     </row>
     <row r="14" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="62"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E14" s="19"/>
-      <c r="F14" s="83" t="s">
-        <v>167</v>
-      </c>
-      <c r="H14" s="74">
+      <c r="F14" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="H14" s="69">
         <v>21</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K14" s="19"/>
-      <c r="L14" s="82" t="s">
-        <v>167</v>
+      <c r="L14" s="77" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="62"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E15" s="19"/>
-      <c r="F15" s="83">
+      <c r="F15" s="78">
         <v>26</v>
       </c>
-      <c r="H15" s="74">
+      <c r="H15" s="69">
         <v>20</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K15" s="19"/>
-      <c r="L15" s="82">
+      <c r="L15" s="77">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="62"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="37"/>
-      <c r="H16" s="74">
+      <c r="H16" s="69">
         <v>19</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="62"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="37"/>
-      <c r="H17" s="76">
+      <c r="H17" s="71">
         <v>18</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K17" s="17"/>
     </row>
     <row r="18" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="80"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="15"/>
       <c r="D18" s="19"/>
       <c r="E18" s="17"/>
@@ -3286,26 +3271,26 @@
       <c r="K18" s="17"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="79"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="37"/>
       <c r="H19" s="24"/>
       <c r="I19" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K19" s="17"/>
     </row>
     <row r="20" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="79"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
       <c r="E20" s="23"/>
@@ -3366,23 +3351,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="A2" s="81" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3395,19 +3380,19 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="D4" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="E4" s="25" t="s">
         <v>119</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3415,13 +3400,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" s="27"/>
     </row>
@@ -3430,13 +3415,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E6" s="27"/>
     </row>
@@ -3448,10 +3433,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E7" s="27"/>
     </row>
@@ -3460,13 +3445,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" s="27"/>
     </row>
@@ -3478,10 +3463,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" s="27"/>
     </row>
@@ -3490,13 +3475,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" s="27"/>
     </row>
@@ -3508,10 +3493,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E11" s="27"/>
     </row>
@@ -3520,13 +3505,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E12" s="29"/>
     </row>
@@ -3538,10 +3523,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E13" s="29"/>
     </row>
@@ -3550,13 +3535,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E14" s="27"/>
     </row>
@@ -3565,13 +3550,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E15" s="27"/>
     </row>
@@ -3580,13 +3565,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E16" s="27"/>
     </row>
@@ -3595,13 +3580,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E17" s="27"/>
     </row>
@@ -3610,13 +3595,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E18" s="29"/>
     </row>
@@ -3628,10 +3613,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E19" s="29"/>
     </row>
@@ -3640,13 +3625,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E20" s="29"/>
     </row>
@@ -3658,10 +3643,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E21" s="29"/>
     </row>
@@ -3670,13 +3655,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E22" s="27"/>
     </row>
@@ -3685,13 +3670,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E23" s="27"/>
     </row>
@@ -3700,13 +3685,13 @@
         <v>19</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E24" s="27"/>
     </row>
@@ -3715,13 +3700,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E25" s="27"/>
     </row>
@@ -3730,13 +3715,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E26" s="27"/>
     </row>
@@ -3745,13 +3730,13 @@
         <v>22</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E27" s="27"/>
     </row>
@@ -3760,13 +3745,13 @@
         <v>23</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E28" s="27"/>
     </row>
@@ -3775,7 +3760,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
@@ -3786,7 +3771,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
@@ -3826,23 +3811,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="A2" s="81" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3855,19 +3840,19 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="D4" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="E4" s="25" t="s">
         <v>119</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3883,7 +3868,7 @@
         <v>Left Drive Victors 1&amp;2 (J1 &amp; J2)</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E5" s="31"/>
     </row>
@@ -3900,7 +3885,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E6" s="27"/>
     </row>
@@ -3917,7 +3902,7 @@
         <v>Right Drive Victor 3&amp;4 (J3 &amp; J4)</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E7" s="27"/>
     </row>
@@ -3934,7 +3919,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E8" s="27"/>
     </row>
@@ -3951,7 +3936,7 @@
         <v>Arm Talon s1 (J5 &amp; J6)</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E9" s="27"/>
     </row>
@@ -3968,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E10" s="27"/>
     </row>
@@ -3985,7 +3970,7 @@
         <v>Shooter Jag</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E11" s="29"/>
     </row>
@@ -4002,7 +3987,7 @@
         <v>Pickup Jag</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E12" s="27"/>
     </row>
@@ -4019,7 +4004,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E13" s="27"/>
     </row>
@@ -4036,7 +4021,7 @@
         <v>indexer Jag</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E14" s="27"/>
     </row>
@@ -4053,7 +4038,7 @@
         <v>Left Drive Enc A</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E15" s="27"/>
     </row>
@@ -4070,7 +4055,7 @@
         <v>Left Drive Enc B</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E16" s="27"/>
     </row>
@@ -4087,7 +4072,7 @@
         <v>Right Drive Enc A</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E17" s="27"/>
     </row>
@@ -4104,7 +4089,7 @@
         <v>Right Drive Enc B</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E18" s="27"/>
     </row>
@@ -4121,7 +4106,7 @@
         <v>Green Claw (1) Lock Sensor</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E19" s="27"/>
     </row>
@@ -4138,7 +4123,7 @@
         <v>Yellow Claw (2) Lock Sensor</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E20" s="27"/>
     </row>
@@ -4155,7 +4140,7 @@
         <v>Indexer SW</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E21" s="27"/>
     </row>
@@ -4172,7 +4157,7 @@
         <v>Compressor Pressure SW</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E22" s="27"/>
     </row>
@@ -4189,7 +4174,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E23" s="29"/>
     </row>
@@ -4206,7 +4191,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E24" s="29"/>
     </row>
@@ -4214,16 +4199,16 @@
       <c r="A25" s="28">
         <v>21</v>
       </c>
-      <c r="B25" s="27" t="str">
+      <c r="B25" s="27">
         <f>'Digital Side Car'!I18</f>
-        <v>DIO11</v>
-      </c>
-      <c r="C25" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C25" s="27">
         <f>'Digital Side Car'!J18</f>
-        <v>Shooter Encoder A</v>
+        <v>0</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E25" s="29"/>
     </row>
@@ -4231,16 +4216,16 @@
       <c r="A26" s="28">
         <v>22</v>
       </c>
-      <c r="B26" s="27" t="str">
+      <c r="B26" s="27">
         <f>'Digital Side Car'!I17</f>
-        <v>DIO12</v>
-      </c>
-      <c r="C26" s="27" t="str">
+        <v>0</v>
+      </c>
+      <c r="C26" s="27">
         <f>'Digital Side Car'!J17</f>
-        <v>Shooter Encoder B</v>
+        <v>0</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E26" s="29"/>
     </row>
@@ -4257,7 +4242,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E27" s="29"/>
     </row>
@@ -4274,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E28" s="27"/>
     </row>
@@ -4291,7 +4276,7 @@
         <v>Shooter Indexer Spike (M1)</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E29" s="27"/>
     </row>
@@ -4308,7 +4293,7 @@
         <v>Compressor motor spike</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E30" s="27"/>
     </row>
@@ -4325,7 +4310,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E31" s="27"/>
     </row>
@@ -4342,7 +4327,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E32" s="29"/>
     </row>
@@ -4359,7 +4344,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E33" s="27"/>
     </row>
@@ -4376,7 +4361,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E34" s="27"/>
     </row>
@@ -4393,7 +4378,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E35" s="27"/>
     </row>
@@ -4410,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E36" s="27"/>
     </row>
@@ -4427,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E37" s="27"/>
     </row>
@@ -4444,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E38" s="27"/>
     </row>
@@ -4461,7 +4446,7 @@
         <v>Shifter A</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E39" s="29"/>
     </row>
@@ -4478,7 +4463,7 @@
         <v>Shifter B</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E40" s="27"/>
     </row>
@@ -4495,7 +4480,7 @@
         <v>Green Claw (1) A</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E41" s="27"/>
     </row>
@@ -4512,7 +4497,7 @@
         <v>Green Claw (2) B</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E42" s="27"/>
     </row>
@@ -4529,7 +4514,7 @@
         <v>Yellow Claw (2) A</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E43" s="27"/>
     </row>
@@ -4546,7 +4531,7 @@
         <v>Yellow Claw (2) B</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E44" s="27"/>
     </row>
@@ -4587,18 +4572,18 @@
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" s="24" t="s">
         <v>143</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4606,43 +4591,43 @@
         <v>5</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D57" s="24" t="s">
         <v>148</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" s="24" t="s">
         <v>151</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D58" s="24" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wiring corrections for PDB.
</commit_message>
<xml_diff>
--- a/2013_Wiring.xlsx
+++ b/2013_Wiring.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="666" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" tabRatio="666"/>
   </bookViews>
   <sheets>
     <sheet name="Power Distribution Board" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="180">
   <si>
     <t>2013 TEAM 2994</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Shooter Jag (J7)</t>
   </si>
   <si>
-    <t>Indexer Spike (M1)</t>
-  </si>
-  <si>
     <t>30A-1</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>30A-6</t>
   </si>
   <si>
-    <t>30A-12</t>
-  </si>
-  <si>
     <t>12V Out</t>
   </si>
   <si>
@@ -526,31 +520,52 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Compressor</t>
-  </si>
-  <si>
-    <t>Left Drive M/C 2 (J2)</t>
-  </si>
-  <si>
-    <t>Right Drive M/c 4 (J4)</t>
-  </si>
-  <si>
-    <t>Right Arm M/C 2(J6)</t>
-  </si>
-  <si>
-    <t>Collector M/C (J8)</t>
-  </si>
-  <si>
-    <t>Left Drive M/C 1 (J1)</t>
-  </si>
-  <si>
-    <t>Right Drive M/C 3 (J3)</t>
-  </si>
-  <si>
-    <t>Left Arm M/C (J5)</t>
-  </si>
-  <si>
-    <t>Shooter M/C (J7)</t>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>J - Jaguar</t>
+  </si>
+  <si>
+    <t>V - Victor</t>
+  </si>
+  <si>
+    <t>U - Variable</t>
+  </si>
+  <si>
+    <t>M/C - Motor Controller</t>
+  </si>
+  <si>
+    <t>Shooter V M/C (J7)</t>
+  </si>
+  <si>
+    <t>Collector J M/C (J8)</t>
+  </si>
+  <si>
+    <t>Indexer J M/C (M1)</t>
+  </si>
+  <si>
+    <t>Compressor Spike</t>
+  </si>
+  <si>
+    <t>20A-12</t>
+  </si>
+  <si>
+    <t>Right Drive 1 V M/C (J3)</t>
+  </si>
+  <si>
+    <t>Right Drive V M/C 2 (J4)</t>
+  </si>
+  <si>
+    <t>Left Drive V 2 M/C (J2)</t>
+  </si>
+  <si>
+    <t>Left Drive 1 V M/C (J1)</t>
+  </si>
+  <si>
+    <t>Arm 2 U M/C (J6)</t>
+  </si>
+  <si>
+    <t>Arm 1 U M/C (J5)</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1093,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1210,8 +1225,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1269,6 +1282,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1921,10 +1939,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,16 +1958,18 @@
     <col min="10" max="10" width="8.5703125"/>
     <col min="11" max="11" width="22" customWidth="1"/>
     <col min="12" max="12" width="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="1022" width="8.5703125"/>
+    <col min="13" max="13" width="8.5703125"/>
+    <col min="14" max="14" width="27.7109375" customWidth="1"/>
+    <col min="15" max="1022" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1957,118 +1977,165 @@
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="54" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="84"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="52"/>
       <c r="C4" s="46"/>
-      <c r="D4" s="35"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
       <c r="J4" s="46"/>
       <c r="K4" s="47"/>
     </row>
-    <row r="5" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="79" t="s">
+    <row r="5" spans="1:15" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="35"/>
-      <c r="J5" s="80" t="s">
+      <c r="C5" s="77"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="80"/>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="78"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
-      <c r="D6" s="35"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
       <c r="J6" s="37"/>
       <c r="K6" s="48"/>
       <c r="L6" s="56" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="57">
         <v>31</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C7" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
       <c r="J7" s="49" t="s">
         <v>5</v>
       </c>
       <c r="K7" s="50" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="L7" s="57">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="82" t="s">
+        <v>164</v>
+      </c>
+      <c r="O7" s="82"/>
+    </row>
+    <row r="8" spans="1:15" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="57">
         <v>30</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C8" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
       <c r="J8" s="49" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="50" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L8" s="57">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="O8" s="82"/>
+    </row>
+    <row r="9" spans="1:15" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="57">
         <v>29</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C9" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
       <c r="J9" s="49" t="s">
         <v>12</v>
       </c>
       <c r="K9" s="50" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="L9" s="57">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N9" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="O9" s="82"/>
+    </row>
+    <row r="10" spans="1:15" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="57">
         <v>28</v>
       </c>
@@ -2078,173 +2145,222 @@
       <c r="C10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
       <c r="J10" s="49" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="51" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="L10" s="57">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="83" t="s">
+        <v>167</v>
+      </c>
+      <c r="O10" s="83"/>
+    </row>
+    <row r="11" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="57">
         <v>27</v>
       </c>
       <c r="B11" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="49" t="s">
         <v>18</v>
-      </c>
-      <c r="D11" s="35"/>
-      <c r="J11" s="49" t="s">
-        <v>19</v>
       </c>
       <c r="K11" s="50"/>
       <c r="L11" s="57"/>
-    </row>
-    <row r="12" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="83" t="s">
+        <v>168</v>
+      </c>
+      <c r="O11" s="83"/>
+    </row>
+    <row r="12" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="57"/>
       <c r="B12" s="55"/>
       <c r="C12" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="49" t="s">
         <v>20</v>
-      </c>
-      <c r="D12" s="35"/>
-      <c r="J12" s="49" t="s">
-        <v>21</v>
       </c>
       <c r="K12" s="50"/>
       <c r="L12" s="57"/>
     </row>
-    <row r="13" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="57"/>
       <c r="B13" s="55"/>
       <c r="C13" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="49" t="s">
         <v>22</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="J13" s="49" t="s">
-        <v>23</v>
       </c>
       <c r="K13" s="50"/>
       <c r="L13" s="57"/>
     </row>
-    <row r="14" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="57">
         <v>26</v>
       </c>
       <c r="B14" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="49" t="s">
         <v>25</v>
-      </c>
-      <c r="D14" s="35"/>
-      <c r="J14" s="49" t="s">
-        <v>26</v>
       </c>
       <c r="K14" s="50"/>
       <c r="L14" s="57"/>
     </row>
-    <row r="15" spans="1:12" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="57">
         <v>25</v>
       </c>
       <c r="B15" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="49" t="s">
         <v>28</v>
-      </c>
-      <c r="D15" s="35"/>
-      <c r="J15" s="49" t="s">
-        <v>29</v>
       </c>
       <c r="K15" s="50"/>
       <c r="L15" s="57"/>
     </row>
-    <row r="16" spans="1:12" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="58">
         <v>24</v>
       </c>
       <c r="B16" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="61"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="64" t="s">
-        <v>166</v>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="82"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="K16" s="62" t="s">
+        <v>172</v>
       </c>
       <c r="L16" s="58">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
-      <c r="D17" s="48"/>
-    </row>
-    <row r="18" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+    </row>
+    <row r="18" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
       <c r="D18" s="48"/>
       <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
       <c r="D19" s="48"/>
       <c r="E19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:9" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
       <c r="D20" s="37"/>
-      <c r="E20" s="76">
+      <c r="E20" s="74">
         <v>38</v>
       </c>
-      <c r="F20" s="76">
+      <c r="F20" s="74">
         <v>37</v>
       </c>
-      <c r="G20" s="76" t="s">
+      <c r="G20" s="74" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="D3:I17"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="J5:K5"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -2263,8 +2379,8 @@
   </sheetPr>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,14 +2400,14 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="45"/>
@@ -2303,7 +2419,7 @@
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
       <c r="G2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H2" s="42"/>
     </row>
@@ -2378,54 +2494,54 @@
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
-      <c r="K14" s="68" t="s">
-        <v>165</v>
+      <c r="K14" s="66" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="68" t="s">
-        <v>165</v>
+      <c r="A15" s="66" t="s">
+        <v>163</v>
       </c>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
       <c r="D15" s="43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="65"/>
-      <c r="K15" s="69"/>
+        <v>42</v>
+      </c>
+      <c r="J15" s="63"/>
+      <c r="K15" s="67"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="69">
+      <c r="A16" s="67">
         <v>6</v>
       </c>
-      <c r="B16" s="66" t="s">
-        <v>157</v>
+      <c r="B16" s="64" t="s">
+        <v>155</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="65"/>
-      <c r="K16" s="69"/>
+        <v>44</v>
+      </c>
+      <c r="J16" s="63"/>
+      <c r="K16" s="67"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="70"/>
+      <c r="A17" s="68"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
       <c r="D17" s="35"/>
@@ -2434,8 +2550,8 @@
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="40"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="72"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="70"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30"/>
@@ -2447,27 +2563,27 @@
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="40"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="72"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="70"/>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="69"/>
-      <c r="B19" s="66"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="37"/>
       <c r="G19" s="37"/>
       <c r="H19" s="37"/>
       <c r="I19" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="J19" s="65"/>
-      <c r="K19" s="69"/>
+        <v>51</v>
+      </c>
+      <c r="J19" s="63"/>
+      <c r="K19" s="67"/>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26"/>
@@ -2479,40 +2595,40 @@
       <c r="G20" s="37"/>
       <c r="H20" s="37"/>
       <c r="I20" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" s="65"/>
-      <c r="K20" s="69"/>
+        <v>54</v>
+      </c>
+      <c r="J20" s="63"/>
+      <c r="K20" s="67"/>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="69">
+      <c r="A21" s="67">
         <v>5</v>
       </c>
-      <c r="B21" s="66" t="s">
-        <v>47</v>
+      <c r="B21" s="64" t="s">
+        <v>45</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E21" s="37"/>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
       <c r="H21" s="37"/>
       <c r="I21" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="J21" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="K21" s="69">
+        <v>56</v>
+      </c>
+      <c r="J21" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="K21" s="67">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="70"/>
+      <c r="A22" s="68"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
       <c r="D22" s="37"/>
@@ -2521,12 +2637,12 @@
       <c r="G22" s="37"/>
       <c r="H22" s="37"/>
       <c r="I22" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="J22" s="65" t="s">
-        <v>62</v>
-      </c>
-      <c r="K22" s="69">
+        <v>59</v>
+      </c>
+      <c r="J22" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="K22" s="67">
         <v>15</v>
       </c>
     </row>
@@ -2540,44 +2656,44 @@
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
       <c r="I23" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="J23" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="K23" s="69">
+        <v>62</v>
+      </c>
+      <c r="J23" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="K23" s="67">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="69">
+      <c r="A24" s="67">
         <v>4</v>
       </c>
-      <c r="B24" s="67" t="s">
-        <v>49</v>
+      <c r="B24" s="65" t="s">
+        <v>47</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
       <c r="G24" s="37"/>
       <c r="H24" s="37"/>
       <c r="I24" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="J24" s="65" t="s">
-        <v>158</v>
-      </c>
-      <c r="K24" s="69">
+        <v>64</v>
+      </c>
+      <c r="J24" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="K24" s="67">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="70"/>
+      <c r="A25" s="68"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
@@ -2586,12 +2702,12 @@
       <c r="G25" s="37"/>
       <c r="H25" s="37"/>
       <c r="I25" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="J25" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="K25" s="72">
+        <v>65</v>
+      </c>
+      <c r="J25" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="K25" s="70">
         <v>82</v>
       </c>
     </row>
@@ -2605,40 +2721,40 @@
       <c r="G26" s="37"/>
       <c r="H26" s="37"/>
       <c r="I26" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="J26" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="K26" s="72">
+        <v>67</v>
+      </c>
+      <c r="J26" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="70">
         <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="69"/>
-      <c r="B27" s="66"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="64"/>
       <c r="C27" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27" s="37"/>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
       <c r="H27" s="37"/>
       <c r="I27" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="J27" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="K27" s="72">
+        <v>69</v>
+      </c>
+      <c r="J27" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" s="70">
         <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="70"/>
+      <c r="A28" s="68"/>
       <c r="B28" s="37"/>
       <c r="C28" s="37"/>
       <c r="D28" s="37"/>
@@ -2647,12 +2763,12 @@
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
       <c r="I28" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="J28" s="65" t="s">
-        <v>74</v>
-      </c>
-      <c r="K28" s="73">
+        <v>71</v>
+      </c>
+      <c r="J28" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="K28" s="71">
         <v>91</v>
       </c>
     </row>
@@ -2668,17 +2784,17 @@
       <c r="K29" s="24"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="69">
+      <c r="A30" s="67">
         <v>3</v>
       </c>
-      <c r="B30" s="66" t="s">
-        <v>156</v>
+      <c r="B30" s="64" t="s">
+        <v>154</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E30" s="37"/>
       <c r="F30" s="37"/>
@@ -2698,26 +2814,26 @@
       <c r="K31" s="24"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="69"/>
-      <c r="B32" s="66"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E32" s="37"/>
       <c r="F32" s="37"/>
       <c r="G32" s="37"/>
       <c r="H32" s="37"/>
       <c r="I32" s="40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J32" s="7"/>
-      <c r="K32" s="68"/>
+      <c r="K32" s="66"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70"/>
+      <c r="A33" s="68"/>
       <c r="B33" s="35"/>
       <c r="C33" s="35"/>
       <c r="D33" s="35"/>
@@ -2726,10 +2842,10 @@
       <c r="G33" s="37"/>
       <c r="H33" s="37"/>
       <c r="I33" s="40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J33" s="7"/>
-      <c r="K33" s="69"/>
+      <c r="K33" s="67"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30"/>
@@ -2741,36 +2857,36 @@
       <c r="G34" s="37"/>
       <c r="H34" s="37"/>
       <c r="I34" s="40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J34" s="7"/>
-      <c r="K34" s="69"/>
+      <c r="K34" s="67"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="69">
+      <c r="A35" s="67">
         <v>2</v>
       </c>
-      <c r="B35" s="66" t="s">
-        <v>155</v>
+      <c r="B35" s="64" t="s">
+        <v>153</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E35" s="37"/>
       <c r="F35" s="37"/>
       <c r="G35" s="37"/>
       <c r="H35" s="37"/>
       <c r="I35" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J35" s="7"/>
-      <c r="K35" s="69"/>
+      <c r="K35" s="67"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="70"/>
+      <c r="A36" s="68"/>
       <c r="B36" s="35"/>
       <c r="C36" s="35"/>
       <c r="D36" s="35"/>
@@ -2779,10 +2895,10 @@
       <c r="G36" s="37"/>
       <c r="H36" s="37"/>
       <c r="I36" s="40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J36" s="7"/>
-      <c r="K36" s="69"/>
+      <c r="K36" s="67"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30"/>
@@ -2794,36 +2910,36 @@
       <c r="G37" s="37"/>
       <c r="H37" s="37"/>
       <c r="I37" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J37" s="7"/>
-      <c r="K37" s="69"/>
+      <c r="K37" s="67"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="69"/>
-      <c r="B38" s="66"/>
+      <c r="A38" s="67"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E38" s="37"/>
       <c r="F38" s="37"/>
       <c r="G38" s="37"/>
       <c r="H38" s="37"/>
       <c r="I38" s="40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="K38" s="69">
+        <v>80</v>
+      </c>
+      <c r="K38" s="67">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="70"/>
+      <c r="A39" s="68"/>
       <c r="B39" s="35"/>
       <c r="C39" s="35"/>
       <c r="D39" s="35"/>
@@ -2832,12 +2948,12 @@
       <c r="G39" s="37"/>
       <c r="H39" s="37"/>
       <c r="I39" s="40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K39" s="71">
+        <v>82</v>
+      </c>
+      <c r="K39" s="69">
         <v>7</v>
       </c>
     </row>
@@ -2852,17 +2968,17 @@
       <c r="H40" s="37"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="71">
+      <c r="A41" s="69">
         <v>1</v>
       </c>
-      <c r="B41" s="66" t="s">
-        <v>154</v>
+      <c r="B41" s="64" t="s">
+        <v>152</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E41" s="37"/>
       <c r="F41" s="37"/>
@@ -2940,25 +3056,25 @@
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.25">
       <c r="F53" s="41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G53" s="41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F54" s="41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G54" s="41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="55" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F55" s="76">
+      <c r="F55" s="74">
         <v>24</v>
       </c>
-      <c r="G55" s="76">
+      <c r="G55" s="74">
         <v>39</v>
       </c>
     </row>
@@ -2999,46 +3115,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
+      <c r="B2" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
       <c r="N2" s="8"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="82" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
+      <c r="C4" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="44"/>
       <c r="I4" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="44"/>
       <c r="K4" s="44"/>
@@ -3046,10 +3162,10 @@
     <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="37"/>
@@ -3060,10 +3176,10 @@
     </row>
     <row r="7" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="37"/>
@@ -3075,7 +3191,7 @@
     <row r="8" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="18"/>
       <c r="D8" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="37"/>
@@ -3086,14 +3202,14 @@
     </row>
     <row r="9" spans="2:14" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="56" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
       <c r="E9" s="17"/>
       <c r="F9" s="37"/>
-      <c r="H9" s="68" t="s">
-        <v>165</v>
+      <c r="H9" s="66" t="s">
+        <v>163</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="19"/>
@@ -3102,17 +3218,17 @@
     <row r="10" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="57"/>
       <c r="C10" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="37"/>
-      <c r="H10" s="69"/>
+      <c r="H10" s="67"/>
       <c r="I10" s="5"/>
       <c r="J10" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K10" s="17"/>
     </row>
@@ -3120,14 +3236,14 @@
       <c r="B11" s="57"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="37"/>
-      <c r="H11" s="69"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="5"/>
       <c r="J11" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K11" s="17"/>
     </row>
@@ -3135,18 +3251,18 @@
       <c r="B12" s="57"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="37"/>
-      <c r="H12" s="69">
+      <c r="H12" s="67">
         <v>23</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K12" s="17"/>
     </row>
@@ -3155,21 +3271,21 @@
         <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="37"/>
-      <c r="H13" s="69">
+      <c r="H13" s="67">
         <v>22</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K13" s="17"/>
     </row>
@@ -3177,47 +3293,47 @@
       <c r="B14" s="57"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E14" s="19"/>
-      <c r="F14" s="78" t="s">
-        <v>165</v>
-      </c>
-      <c r="H14" s="69">
+      <c r="F14" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="H14" s="67">
         <v>21</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K14" s="19"/>
-      <c r="L14" s="77" t="s">
-        <v>165</v>
+      <c r="L14" s="75" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="57"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E15" s="19"/>
-      <c r="F15" s="78">
+      <c r="F15" s="76">
         <v>26</v>
       </c>
-      <c r="H15" s="69">
+      <c r="H15" s="67">
         <v>20</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K15" s="19"/>
-      <c r="L15" s="77">
+      <c r="L15" s="75">
         <v>25</v>
       </c>
     </row>
@@ -3225,18 +3341,18 @@
       <c r="B16" s="57"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="37"/>
-      <c r="H16" s="69">
+      <c r="H16" s="67">
         <v>19</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K16" s="17"/>
     </row>
@@ -3244,23 +3360,23 @@
       <c r="B17" s="57"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="37"/>
-      <c r="H17" s="71">
+      <c r="H17" s="69">
         <v>18</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K17" s="17"/>
     </row>
     <row r="18" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="75"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="15"/>
       <c r="D18" s="19"/>
       <c r="E18" s="17"/>
@@ -3271,26 +3387,26 @@
       <c r="K18" s="17"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="74"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="37"/>
       <c r="H19" s="24"/>
       <c r="I19" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K19" s="17"/>
     </row>
     <row r="20" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="74"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
       <c r="E20" s="23"/>
@@ -3351,23 +3467,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
+      <c r="A2" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3380,19 +3496,19 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="D4" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="E4" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3400,13 +3516,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E5" s="27"/>
     </row>
@@ -3415,13 +3531,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E6" s="27"/>
     </row>
@@ -3433,10 +3549,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E7" s="27"/>
     </row>
@@ -3445,13 +3561,13 @@
         <v>3</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E8" s="27"/>
     </row>
@@ -3463,10 +3579,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E9" s="27"/>
     </row>
@@ -3475,13 +3591,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E10" s="27"/>
     </row>
@@ -3493,10 +3609,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E11" s="27"/>
     </row>
@@ -3505,13 +3621,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E12" s="29"/>
     </row>
@@ -3523,10 +3639,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E13" s="29"/>
     </row>
@@ -3535,13 +3651,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E14" s="27"/>
     </row>
@@ -3550,13 +3666,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E15" s="27"/>
     </row>
@@ -3565,13 +3681,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E16" s="27"/>
     </row>
@@ -3580,13 +3696,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E17" s="27"/>
     </row>
@@ -3595,13 +3711,13 @@
         <v>13</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E18" s="29"/>
     </row>
@@ -3613,10 +3729,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E19" s="29"/>
     </row>
@@ -3625,13 +3741,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E20" s="29"/>
     </row>
@@ -3643,10 +3759,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E21" s="29"/>
     </row>
@@ -3655,13 +3771,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E22" s="27"/>
     </row>
@@ -3670,13 +3786,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E23" s="27"/>
     </row>
@@ -3685,13 +3801,13 @@
         <v>19</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E24" s="27"/>
     </row>
@@ -3700,13 +3816,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E25" s="27"/>
     </row>
@@ -3715,13 +3831,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E26" s="27"/>
     </row>
@@ -3730,13 +3846,13 @@
         <v>22</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E27" s="27"/>
     </row>
@@ -3745,13 +3861,13 @@
         <v>23</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E28" s="27"/>
     </row>
@@ -3760,7 +3876,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
@@ -3771,7 +3887,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
@@ -3811,23 +3927,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
+      <c r="A2" s="79" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3840,19 +3956,19 @@
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="D4" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="E4" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3868,7 +3984,7 @@
         <v>Left Drive Victors 1&amp;2 (J1 &amp; J2)</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E5" s="31"/>
     </row>
@@ -3885,7 +4001,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E6" s="27"/>
     </row>
@@ -3902,7 +4018,7 @@
         <v>Right Drive Victor 3&amp;4 (J3 &amp; J4)</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E7" s="27"/>
     </row>
@@ -3919,7 +4035,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E8" s="27"/>
     </row>
@@ -3936,7 +4052,7 @@
         <v>Arm Talon s1 (J5 &amp; J6)</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E9" s="27"/>
     </row>
@@ -3953,7 +4069,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E10" s="27"/>
     </row>
@@ -3970,7 +4086,7 @@
         <v>Shooter Jag</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E11" s="29"/>
     </row>
@@ -3987,7 +4103,7 @@
         <v>Pickup Jag</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E12" s="27"/>
     </row>
@@ -4004,7 +4120,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E13" s="27"/>
     </row>
@@ -4021,7 +4137,7 @@
         <v>indexer Jag</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E14" s="27"/>
     </row>
@@ -4038,7 +4154,7 @@
         <v>Left Drive Enc A</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E15" s="27"/>
     </row>
@@ -4055,7 +4171,7 @@
         <v>Left Drive Enc B</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E16" s="27"/>
     </row>
@@ -4072,7 +4188,7 @@
         <v>Right Drive Enc A</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E17" s="27"/>
     </row>
@@ -4089,7 +4205,7 @@
         <v>Right Drive Enc B</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E18" s="27"/>
     </row>
@@ -4106,7 +4222,7 @@
         <v>Green Claw (1) Lock Sensor</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E19" s="27"/>
     </row>
@@ -4123,7 +4239,7 @@
         <v>Yellow Claw (2) Lock Sensor</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E20" s="27"/>
     </row>
@@ -4140,7 +4256,7 @@
         <v>Indexer SW</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E21" s="27"/>
     </row>
@@ -4157,7 +4273,7 @@
         <v>Compressor Pressure SW</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E22" s="27"/>
     </row>
@@ -4174,7 +4290,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E23" s="29"/>
     </row>
@@ -4191,7 +4307,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E24" s="29"/>
     </row>
@@ -4208,7 +4324,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E25" s="29"/>
     </row>
@@ -4225,7 +4341,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E26" s="29"/>
     </row>
@@ -4242,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E27" s="29"/>
     </row>
@@ -4259,7 +4375,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E28" s="27"/>
     </row>
@@ -4276,7 +4392,7 @@
         <v>Shooter Indexer Spike (M1)</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E29" s="27"/>
     </row>
@@ -4293,7 +4409,7 @@
         <v>Compressor motor spike</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E30" s="27"/>
     </row>
@@ -4310,7 +4426,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E31" s="27"/>
     </row>
@@ -4327,7 +4443,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E32" s="29"/>
     </row>
@@ -4344,7 +4460,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E33" s="27"/>
     </row>
@@ -4361,7 +4477,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E34" s="27"/>
     </row>
@@ -4378,7 +4494,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E35" s="27"/>
     </row>
@@ -4395,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E36" s="27"/>
     </row>
@@ -4412,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E37" s="27"/>
     </row>
@@ -4429,7 +4545,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E38" s="27"/>
     </row>
@@ -4446,7 +4562,7 @@
         <v>Shifter A</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E39" s="29"/>
     </row>
@@ -4463,7 +4579,7 @@
         <v>Shifter B</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E40" s="27"/>
     </row>
@@ -4480,7 +4596,7 @@
         <v>Green Claw (1) A</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E41" s="27"/>
     </row>
@@ -4497,7 +4613,7 @@
         <v>Green Claw (2) B</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E42" s="27"/>
     </row>
@@ -4514,7 +4630,7 @@
         <v>Yellow Claw (2) A</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E43" s="27"/>
     </row>
@@ -4531,7 +4647,7 @@
         <v>Yellow Claw (2) B</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E44" s="27"/>
     </row>
@@ -4572,18 +4688,18 @@
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="D55" s="24" t="s">
         <v>141</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4591,43 +4707,43 @@
         <v>5</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" s="24" t="s">
         <v>146</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D58" s="24" t="s">
         <v>149</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D58" s="24" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final updates by Dan
</commit_message>
<xml_diff>
--- a/2013_Wiring.xlsx
+++ b/2013_Wiring.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="12660" tabRatio="666" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="12660" tabRatio="666" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Power Distribution Board" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="193">
   <si>
     <t>2013 TEAM 2994</t>
   </si>
@@ -581,16 +581,25 @@
     <t>Shooter Motor Controller</t>
   </si>
   <si>
-    <t>Left Drive Motor Controllers</t>
-  </si>
-  <si>
-    <t>Right Drive Motor Controllers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Arm Motor Controllers </t>
   </si>
   <si>
     <t>indexer Motor Controller</t>
+  </si>
+  <si>
+    <t>Left Drive Bottom Motor Cont.</t>
+  </si>
+  <si>
+    <t>Left Drive Top Motor Cont.</t>
+  </si>
+  <si>
+    <t>Right Drive Top Motor Cont.</t>
+  </si>
+  <si>
+    <t>Right Drive Bottom Motor Cont.</t>
+  </si>
+  <si>
+    <t>Ammeter</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1419,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1031" name="Picture 3"/>
+        <xdr:cNvPr id="2049" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1563,20 +1572,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2066925</xdr:colOff>
+      <xdr:colOff>2057400</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2051" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1644,7 +1653,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3077" name="Picture 2"/>
+        <xdr:cNvPr id="3073" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1707,7 +1716,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3078" name="Picture 3"/>
+        <xdr:cNvPr id="3074" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2488,13 +2497,13 @@
   </sheetPr>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.5703125" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
@@ -2629,7 +2638,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>40</v>
@@ -2899,7 +2908,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="60" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>51</v>
@@ -2925,8 +2934,12 @@
       <c r="K31" s="24"/>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="63"/>
-      <c r="B32" s="60"/>
+      <c r="A32" s="63">
+        <v>42</v>
+      </c>
+      <c r="B32" s="60" t="s">
+        <v>191</v>
+      </c>
       <c r="C32" s="33" t="s">
         <v>53</v>
       </c>
@@ -2978,7 +2991,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="60" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>56</v>
@@ -3027,8 +3040,12 @@
       <c r="K37" s="63"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="63"/>
-      <c r="B38" s="60"/>
+      <c r="A38" s="63">
+        <v>41</v>
+      </c>
+      <c r="B38" s="60" t="s">
+        <v>188</v>
+      </c>
       <c r="C38" s="33" t="s">
         <v>59</v>
       </c>
@@ -3079,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="60" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>61</v>
@@ -3201,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3464,8 +3481,12 @@
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="53"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="53">
+        <v>44</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="D17" s="6" t="s">
         <v>105</v>
       </c>
@@ -4020,7 +4041,7 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C1:C65536"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,7 +4110,7 @@
       </c>
       <c r="C5" s="31" t="str">
         <f>'Digital Side Car'!B41</f>
-        <v>Left Drive Motor Controllers</v>
+        <v>Left Drive Top Motor Cont.</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>172</v>
@@ -4099,17 +4120,19 @@
     <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27">
         <f>'Digital Side Car'!A38</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B6" s="27" t="str">
         <f>'Digital Side Car'!C38</f>
         <v>PWM2</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="27" t="str">
         <f>'Digital Side Car'!B38</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="27"/>
+        <v>Left Drive Bottom Motor Cont.</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>172</v>
+      </c>
       <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4123,7 +4146,7 @@
       </c>
       <c r="C7" s="27" t="str">
         <f>'Digital Side Car'!B35</f>
-        <v>Right Drive Motor Controllers</v>
+        <v>Right Drive Top Motor Cont.</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>172</v>
@@ -4133,17 +4156,19 @@
     <row r="8" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
         <f>'Digital Side Car'!A32</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B8" s="27" t="str">
         <f>'Digital Side Car'!C32</f>
         <v>PWM4</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="27" t="str">
         <f>'Digital Side Car'!B32</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="27"/>
+        <v>Right Drive Bottom Motor Cont.</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>172</v>
+      </c>
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4591,17 +4616,19 @@
     <row r="35" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27">
         <f>Breakouts!B17</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B35" s="27" t="str">
         <f>Breakouts!D17</f>
         <v>AI1</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="27" t="str">
         <f>Breakouts!C17</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="27"/>
+        <v>Ammeter</v>
+      </c>
+      <c r="D35" s="73" t="s">
+        <v>176</v>
+      </c>
       <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>